<commit_message>
created in memory db and repository and entities, setup commandline runner to insert the data from json files
</commit_message>
<xml_diff>
--- a/woordenlijst.xlsx
+++ b/woordenlijst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>